<commit_message>
Optimisation du code HTML et CSS et début du rapport d'analyse
</commit_message>
<xml_diff>
--- a/Audit SEO.xlsx
+++ b/Audit SEO.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Documents\Formation\Projets\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8910F41C-C031-439C-A44F-4897243541A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="620" windowWidth="27860" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Catégorie</t>
   </si>
@@ -51,12 +52,83 @@
   </si>
   <si>
     <t>(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>SEO / Accessibilité</t>
+  </si>
+  <si>
+    <t>La balise &lt;title&gt; de la page d'accueil est vide</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Certaines polices sont trop petites</t>
+  </si>
+  <si>
+    <t>Anuaire de liens dans le footer</t>
+  </si>
+  <si>
+    <t>Sur la page 2, mauvais chemin JavaScript</t>
+  </si>
+  <si>
+    <t>Mots-clés invisibles placés sur la page</t>
+  </si>
+  <si>
+    <t>Code vide (ex. liste)</t>
+  </si>
+  <si>
+    <t>Images sans équivalent textuel</t>
+  </si>
+  <si>
+    <t>Images sans description</t>
+  </si>
+  <si>
+    <t>Mauvaise structure des titres (h1, h2, etc…)</t>
+  </si>
+  <si>
+    <t>Langue non indiquée dans la balise html</t>
+  </si>
+  <si>
+    <t>WCAG Chapitre 3.1.1
+Language of Page</t>
+  </si>
+  <si>
+    <t>SEO : S'il n'y a pas de titre, Google ne sait pas de quoi parle la page au premier abord et ne la classera sûrement pas bien.
+Accessibilité : Sans titre, une personne aveugle sera par exemple incapable de savoir de quoi parle la page, puisque l'ordinateur ne pourra pas lui lire.</t>
+  </si>
+  <si>
+    <t>Remplir la balise avec un titre qui met en avant les mots-clés importants du site et qui décrit la page</t>
+  </si>
+  <si>
+    <t>WCAG Chapitre 2.4.2
+Page Titled
+Cours SEO OpenClassrooms
+Optimisez le contenu de vos pages.</t>
+  </si>
+  <si>
+    <t>Images trop lourdes</t>
+  </si>
+  <si>
+    <t>Pas de balise &lt;address&gt; pour les coordonnées</t>
+  </si>
+  <si>
+    <t>Titre page 2 en orange sur orange</t>
+  </si>
+  <si>
+    <t>Les textes blancs sur fond orange ne sont pas assez contrastés</t>
+  </si>
+  <si>
+    <t>Elles peuvent être très difficiles à lire pour certaines personnes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -103,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -112,24 +184,231 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,6 +418,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -341,123 +623,282 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="26" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" s="2" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E3" s="4"/>
+    <row r="3" spans="1:26" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E4" s="4"/>
+    <row r="4" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="4"/>
+    <row r="5" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E6" s="4"/>
+    <row r="6" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E7" s="4"/>
+    <row r="7" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E8" s="4"/>
+    <row r="8" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="4"/>
+    <row r="9" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E10" s="4"/>
+    <row r="10" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E11" s="4"/>
+    <row r="11" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E12" s="4"/>
+    <row r="12" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E13" s="4"/>
+    <row r="13" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E14" s="4"/>
+    <row r="14" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E15" s="4"/>
+    <row r="15" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1424,8 +1865,6 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Changement de couleur pour le contraste
</commit_message>
<xml_diff>
--- a/Audit SEO.xlsx
+++ b/Audit SEO.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Documents\Formation\Projets\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8910F41C-C031-439C-A44F-4897243541A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53805B1-CD9A-4317-9EFD-2F1A3E8A2931}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-7140" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>Catégorie</t>
   </si>
@@ -51,57 +51,20 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>(SEO ou accessiblité ?)</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
     <t>SEO / Accessibilité</t>
   </si>
   <si>
-    <t>La balise &lt;title&gt; de la page d'accueil est vide</t>
-  </si>
-  <si>
     <t>Accessibilité</t>
   </si>
   <si>
-    <t>Certaines polices sont trop petites</t>
-  </si>
-  <si>
-    <t>Anuaire de liens dans le footer</t>
-  </si>
-  <si>
-    <t>Sur la page 2, mauvais chemin JavaScript</t>
-  </si>
-  <si>
-    <t>Mots-clés invisibles placés sur la page</t>
-  </si>
-  <si>
-    <t>Code vide (ex. liste)</t>
-  </si>
-  <si>
-    <t>Images sans équivalent textuel</t>
-  </si>
-  <si>
-    <t>Images sans description</t>
-  </si>
-  <si>
     <t>Mauvaise structure des titres (h1, h2, etc…)</t>
-  </si>
-  <si>
-    <t>Langue non indiquée dans la balise html</t>
   </si>
   <si>
     <t>WCAG Chapitre 3.1.1
 Language of Page</t>
-  </si>
-  <si>
-    <t>SEO : S'il n'y a pas de titre, Google ne sait pas de quoi parle la page au premier abord et ne la classera sûrement pas bien.
-Accessibilité : Sans titre, une personne aveugle sera par exemple incapable de savoir de quoi parle la page, puisque l'ordinateur ne pourra pas lui lire.</t>
-  </si>
-  <si>
-    <t>Remplir la balise avec un titre qui met en avant les mots-clés importants du site et qui décrit la page</t>
   </si>
   <si>
     <t>WCAG Chapitre 2.4.2
@@ -110,19 +73,199 @@
 Optimisez le contenu de vos pages.</t>
   </si>
   <si>
-    <t>Images trop lourdes</t>
-  </si>
-  <si>
-    <t>Pas de balise &lt;address&gt; pour les coordonnées</t>
-  </si>
-  <si>
-    <t>Titre page 2 en orange sur orange</t>
-  </si>
-  <si>
-    <t>Les textes blancs sur fond orange ne sont pas assez contrastés</t>
-  </si>
-  <si>
     <t>Elles peuvent être très difficiles à lire pour certaines personnes.</t>
+  </si>
+  <si>
+    <t>Les textes peuvent être difficiles à lire pour certaines personnes.</t>
+  </si>
+  <si>
+    <t>Agrandir les polices d'écritures à 16px au minimum.</t>
+  </si>
+  <si>
+    <t>S'assurer que tous les liens du code fonctionnent.</t>
+  </si>
+  <si>
+    <t>Supprimer ces textes et mettre plutôt les mots-clés dans des paragraphes de manière pertinente.</t>
+  </si>
+  <si>
+    <t>"Nettoyer" le code inutile.</t>
+  </si>
+  <si>
+    <t>Décrire l'image dans le "alt" de la balise.</t>
+  </si>
+  <si>
+    <t>Si possible, remplacer les images qui ne contiennent que du texte par des blocs de texte, sinon écrire le texte en description.</t>
+  </si>
+  <si>
+    <t>Indiquer "fr" dans la balise langue.</t>
+  </si>
+  <si>
+    <t>Les textes sur fond coloré ne sont pas assez contrastés.</t>
+  </si>
+  <si>
+    <t>Remplacer la couleur de police ou de fond, ou appliquer un contour noir ou une ombre sur les polices.</t>
+  </si>
+  <si>
+    <t>Google aura du mal à déterminer la langue de site pour le référencer.
+Certains outils d'accessibilité pourraient penser que le site est en anglais sans précision supplémentaire.</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Officiellement, pas de taille de police minimum.
+16px généralement recommandé :
+https://accessibleweb.com/question-answer/minimum-font-size/</t>
+  </si>
+  <si>
+    <t>Les liens externes n'ont pas de rapport avec le contenu du site et sont considérés comme une pratique Black Hat.
+De plus les liens dans les parties communes aux différentes pages du site ont beaucoup moins d'importance aux yeux de Google.</t>
+  </si>
+  <si>
+    <t>Supprimer les liens dans le footer ou en mettre vers des entreprises partenaires pertinentes.
+L'idéal serait d'en mettre de manière cohérente dans la page directement, et pas dans le footer ou header.</t>
+  </si>
+  <si>
+    <t>Cours OpenClassrooms
+Augmentez l'autorité de votre site.</t>
+  </si>
+  <si>
+    <t>Le footer comporte un "annuaire" de liens.</t>
+  </si>
+  <si>
+    <t>Certaines polices sont trop petites.</t>
+  </si>
+  <si>
+    <t>Les fichiers JavaScript chargés sont lourds et nombreux.</t>
+  </si>
+  <si>
+    <t>Le site risque de dépasser le budget de crawl de Google.</t>
+  </si>
+  <si>
+    <t>Les fichiers JavaScript ne sont pas chargés, cela crée des erreurs sur la page : la page n'est pas fonctionnelle, ni pour l'utilisateur, ni pour Google.</t>
+  </si>
+  <si>
+    <t>Sur la page 2, les chemins des fichiers JavaScript à charger sont incorrects.</t>
+  </si>
+  <si>
+    <t>Cours OpenClassrooms
+Optimisez le SEO de votre site en améliorant ses performances techniques.</t>
+  </si>
+  <si>
+    <t>Ce fichier est un guide pour Googlebot et son absence peut aboutir à des résultats de recherche moins pertinents.</t>
+  </si>
+  <si>
+    <t>Créer un fichier robots.txt et lui indiquer quelles pages Google peut explorer.</t>
+  </si>
+  <si>
+    <t>Documentation Google Developers
+Bonnes pratiques SEO</t>
+  </si>
+  <si>
+    <t>Les pages comportent peu de mots.</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de fichier robots.txt.</t>
+  </si>
+  <si>
+    <t>Il est recommandé d'avoir au moins 1000 mots sur une page.</t>
+  </si>
+  <si>
+    <t>Les pages comportant peu de mots peuvent être moins bien référencées.</t>
+  </si>
+  <si>
+    <t>Seobility.net</t>
+  </si>
+  <si>
+    <t>Optimiser le code JavaScript pour alléger le fichier et tout organiser dans un seul fichier si possible.</t>
+  </si>
+  <si>
+    <t>De nombreux mots clés invisibles placés sur la page.</t>
+  </si>
+  <si>
+    <t>SEO : Cette pratique est considérée comme du Black Hat par Google.
+Accessibilité : Ces mots seraient lu par un lecteur d'écran pour une personne non-voyante par exemple, ce qui n'a ni sens si contexte au milieu d'une page.</t>
+  </si>
+  <si>
+    <t>Google : Consignes aux webmasters
+Mozilla Mobile Accessibility Checklist
+La visibilité</t>
+  </si>
+  <si>
+    <t>Certaines parties du code sont vides et inutiles (ex. liste).</t>
+  </si>
+  <si>
+    <t>Du code inutile rend la page plus longue à charger et à crawler, cela consomme plus de budget et n'apporte rien.</t>
+  </si>
+  <si>
+    <t>Des textes sont placés dans des images.</t>
+  </si>
+  <si>
+    <t>L'image ne peut pas être décrite aux non-voyants et le texte ne se redimensionne pas avec la page.</t>
+  </si>
+  <si>
+    <t>WCAG Chapitres 1.4.5 et 1.4.9
+Images of Text
+Mozilla Mobile Accessibility Checklist
+Les équivalents textuels</t>
+  </si>
+  <si>
+    <t>Des images n'ont pas de description.</t>
+  </si>
+  <si>
+    <t>Accessibilité / SEO</t>
+  </si>
+  <si>
+    <t>Accessibilité : L'image ne peut pas être décrite aux non-voyants.
+SEO : Google ne peut pas interpréter l'image et ne sait pas de quoi il s'agit.</t>
+  </si>
+  <si>
+    <t>WCAG Chapitre 1.1
+Text Alternatives</t>
+  </si>
+  <si>
+    <t>Google :
+SEO pour les débutants
+Consignes aux webmasters</t>
+  </si>
+  <si>
+    <t>Google ne sait pas quels sont les éléments les plus importants de la page, de plus, le robot Google peut se perdre dans le site ce qui est mauvais pour le référencement.</t>
+  </si>
+  <si>
+    <t>Structurer les pages correctement et utiliser les balises de titre pour mettre en avant les termes importants.</t>
+  </si>
+  <si>
+    <t>Aucune langue n'est indiquée dans la balise html.</t>
+  </si>
+  <si>
+    <t>Beaucoup d'images sont trop lourdes.</t>
+  </si>
+  <si>
+    <t>La page est longue à charger, ce qui est désagréable pour l'utilisateur et un mauvais point pour Google, qui peut abandonner le crawling si la page est trop lourde.</t>
+  </si>
+  <si>
+    <t>SearchEngineJournal
+SearchEngineWatch :
+Image optimization for SEO</t>
+  </si>
+  <si>
+    <t>Réduire la résolution des images quand c'est possible, et changer les formats non standard ou moins optimisés (bmp -&gt; jpg par exemple) pour atteindre moins de 200ko pour les grandes images et moins de 100ko pour les petites.</t>
+  </si>
+  <si>
+    <t>WCAG Chapitre 1.4.3
+Contrast
+Mozilla Mobile Accessibility Checklist
+Couleur</t>
+  </si>
+  <si>
+    <t>Les balises &lt;title&gt; et &lt;description&gt; sont vides.</t>
+  </si>
+  <si>
+    <t>Remplir les balises avec un titre et une description qui mettent en avant les mots-clés importants du site et qui décrivent la page.</t>
+  </si>
+  <si>
+    <t>SEO : S'il n'y a pas de titre ni description, Google ne sait pas de quoi parle la page au premier abord et ne la classera sûrement pas bien.
+Accessibilité : Sans titre et description, une personne aveugle sera par exemple incapable de savoir de quoi parle la page, puisque l'ordinateur ne pourra pas lui lire.</t>
   </si>
 </sst>
 </file>
@@ -151,17 +294,19 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,8 +319,13 @@
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -205,51 +355,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -355,11 +460,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -367,25 +488,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -394,24 +515,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -624,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -681,224 +797,312 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="141" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+    <row r="5" spans="1:26" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="C14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
-        <v>23</v>
+      <c r="E14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+    <row r="15" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="9" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+    <row r="16" spans="1:26" ht="73.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1863,8 +2067,6 @@
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>